<commit_message>
New allure-results, new bugs
</commit_message>
<xml_diff>
--- a/Баг-Репорт.xlsx
+++ b/Баг-Репорт.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diplom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F388ADDE-21AB-424F-AA46-6312A40242C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4405FA4-683C-49CB-B247-D1A2AE42525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
   <si>
     <t>Номер дефекта</t>
   </si>
@@ -236,6 +236,24 @@
   </si>
   <si>
     <t>Некорректная отрисовка элементов под темную тему android-устройства</t>
+  </si>
+  <si>
+    <t>Недоступен переход на страницу About со страницы News</t>
+  </si>
+  <si>
+    <t>Вкладка About недоступна для перехода с вкладки News</t>
+  </si>
+  <si>
+    <t>Открылась страница About на которой размещены ссылки на политику конфеденциальности и условия эксплуатации</t>
+  </si>
+  <si>
+    <t>Загрузилась страница с текстом условий эксплуатации ()</t>
+  </si>
+  <si>
+    <t>Вкладка About светлосерая и недоступна для перехода</t>
+  </si>
+  <si>
+    <t>https://disk.yandex.ru/i/4bMhK0TrG0PbJg</t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,94 +567,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -650,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,29 +590,128 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -693,14 +720,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,10 +927,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -933,7 +963,7 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="22" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -950,228 +980,228 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="44">
+      <c r="A2" s="61">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>62</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="66" t="s">
+      <c r="J2" s="54" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="49"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="48"/>
       <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="39"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="49"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="39"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="39"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="55"/>
     </row>
     <row r="6" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="42" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="49"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="39"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="49"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="39"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="1:18" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="49"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="39"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:18" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="49"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="39"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="55"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="50"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="39"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="22">
+      <c r="A11" s="37">
         <v>2</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="37" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="37" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="23"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="39"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="22">
+      <c r="A13" s="37">
         <v>3</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="37" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="66" t="s">
+      <c r="J13" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K13" s="12"/>
@@ -1184,18 +1214,18 @@
       <c r="R13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="23"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="32"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -1206,34 +1236,34 @@
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="35" t="s">
+      <c r="E15" s="66"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="32"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="65"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="32"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="65"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
@@ -1244,354 +1274,450 @@
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="22">
+      <c r="A17" s="37">
         <v>4</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="37" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="37" t="s">
         <v>62</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="66" t="s">
+      <c r="I17" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="54" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="35" t="s">
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="26" t="s">
+      <c r="A19" s="64"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="32"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="65"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="35" t="s">
+      <c r="A20" s="64"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="32"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="65"/>
     </row>
     <row r="21" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="33"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="52"/>
     </row>
     <row r="22" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="22">
+      <c r="A22" s="37">
         <v>5</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="37" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="23"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="53" t="s">
+      <c r="E23" s="45"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="69" t="s">
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="33" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="54" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="70" t="s">
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="73" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="61" t="s">
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="39" t="s">
         <v>66</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="70"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="73"/>
     </row>
     <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="54" t="s">
+      <c r="A26" s="64"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="70"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="73"/>
     </row>
     <row r="27" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="55" t="s">
+      <c r="A27" s="64"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="70"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="73"/>
     </row>
     <row r="28" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="54" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="71"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="74"/>
     </row>
     <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="22">
+      <c r="A29" s="37">
         <v>6</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="37" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="37" t="s">
         <v>62</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J29" s="68" t="s">
+      <c r="J29" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="23"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="69"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="51"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="72"/>
-    </row>
-    <row r="32" spans="1:10" s="57" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="22">
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="34"/>
+    </row>
+    <row r="32" spans="1:10" s="27" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="37">
         <v>7</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="74" t="s">
+      <c r="F32" s="36" t="s">
         <v>68</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="I32" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J32" s="68" t="s">
+      <c r="J32" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="59" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="51"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="58" t="s">
+    <row r="33" spans="1:14" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="38"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="60" t="s">
+      <c r="E33" s="38"/>
+      <c r="F33" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+    </row>
+    <row r="34" spans="1:14" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="37">
+        <v>8</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="45"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="33"/>
+    </row>
+    <row r="36" spans="1:14" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="45"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="33"/>
+    </row>
+    <row r="37" spans="1:14" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="38"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="F2:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="H29:H31"/>
+  <mergeCells count="71">
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="H22:H28"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="H2:H10"/>
     <mergeCell ref="I2:I10"/>
     <mergeCell ref="J2:J10"/>
     <mergeCell ref="A11:A12"/>
@@ -1607,37 +1733,30 @@
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="E2:E10"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="H2:H10"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H13:H16"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="F2:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="H29:H31"/>
     <mergeCell ref="I22:I28"/>
     <mergeCell ref="D24:D28"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="H22:H28"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C34:C998" xr:uid="{00DA00CA-009D-4710-95E6-007E00A90096}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" sqref="C38:C1000" xr:uid="{00DA00CA-009D-4710-95E6-007E00A90096}">
       <formula1>"Блокирующая (Blocker),Критическая (Critical),Средняя (Medium),Низкая (Low)"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2" xr:uid="{0063004C-00B8-4E13-85EA-005500FC0014}">

</xml_diff>